<commit_message>
DOE with 5000 cases
</commit_message>
<xml_diff>
--- a/datasets/DOE_Setup.xlsx
+++ b/datasets/DOE_Setup.xlsx
@@ -517,7 +517,7 @@
         <v>9000</v>
       </c>
       <c r="F5">
-        <v>1000</v>
+        <v>200</v>
       </c>
       <c r="G5">
         <v>0.95</v>
@@ -546,7 +546,7 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2">
-        <v>1000</v>
+        <v>5000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Optimized DOE with 5000 cases
</commit_message>
<xml_diff>
--- a/datasets/DOE_Setup.xlsx
+++ b/datasets/DOE_Setup.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>Variable Name</t>
   </si>
@@ -51,9 +51,6 @@
   </si>
   <si>
     <t>Capacity</t>
-  </si>
-  <si>
-    <t>Continuous</t>
   </si>
   <si>
     <t>Discrete</t>
@@ -453,11 +450,14 @@
       <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2">
-        <v>20</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
+      <c r="D2">
+        <v>30</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0.1</v>
       </c>
       <c r="G2">
         <v>0.95</v>
@@ -471,10 +471,10 @@
         <v>9</v>
       </c>
       <c r="D3">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="E3">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F3">
         <v>0.1</v>
@@ -483,7 +483,7 @@
         <v>0.95</v>
       </c>
       <c r="H3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -503,7 +503,7 @@
         <v>0.95</v>
       </c>
       <c r="H4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -511,19 +511,19 @@
         <v>11</v>
       </c>
       <c r="D5">
-        <v>18000</v>
+        <v>20000</v>
       </c>
       <c r="E5">
-        <v>9000</v>
+        <v>5000</v>
       </c>
       <c r="F5">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="G5">
         <v>0.95</v>
       </c>
       <c r="H5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -541,7 +541,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:1">

</xml_diff>